<commit_message>
Add External Mig Type to InMigration domain
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/ext_inmigration_form.xlsx
+++ b/app/src/main/res/raw/ext_inmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17670" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12270" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -1591,8 +1591,8 @@
   <sheetPr/>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="I6" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Add ExternalInMigration feature (missing extra creation validations)
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/ext_inmigration_form.xlsx
+++ b/app/src/main/res/raw/ext_inmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12270" tabRatio="500"/>
+    <workbookView windowWidth="20850" windowHeight="5160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -585,9 +585,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -627,16 +627,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -657,6 +657,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -672,10 +680,63 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -688,24 +749,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -720,14 +765,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -735,44 +773,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -798,25 +798,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,157 +972,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -996,7 +996,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1005,46 +1005,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1076,164 +1052,188 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1591,8 +1591,8 @@
   <sheetPr/>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="I6" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -2755,7 +2755,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Add support for phone numbers attributes for Member domain - Add variables to ExtInMig/MemberEnu/InMig FormUtils and HDS-Forms - Add variables to Member Details layout and Editor - Add synchronization methods
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/ext_inmigration_form.xlsx
+++ b/app/src/main/res/raw/ext_inmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12240" tabRatio="500"/>
+    <workbookView windowWidth="27795" windowHeight="12195" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="262">
   <si>
     <t>group</t>
   </si>
@@ -394,6 +394,51 @@
     <t>4.7. Religião</t>
   </si>
   <si>
+    <t>hasPhoneNumbers</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>4.8.  Does the member have a phone number?</t>
+  </si>
+  <si>
+    <t>4.8. O membro tem um número de telefone?</t>
+  </si>
+  <si>
+    <t>4.8. Le membre a-t-il un numéro de téléphone?</t>
+  </si>
+  <si>
+    <t>phonePrimary</t>
+  </si>
+  <si>
+    <t>4.8.1. What is the member's primary phone number?</t>
+  </si>
+  <si>
+    <t>4.8.1. Qual é o número de telefone principal do membro?</t>
+  </si>
+  <si>
+    <t>4.8.1. Quel est le numéro de téléphone principal du membre?</t>
+  </si>
+  <si>
+    <t>${hasPhoneNumbers} = 'true'</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>phoneAlternative</t>
+  </si>
+  <si>
+    <t>4.8.2. What is the member's alternative phone number?  (If available)</t>
+  </si>
+  <si>
+    <t>4.8.2. Qual é o número de telefone alternativo do membro? (Se disponível)</t>
+  </si>
+  <si>
+    <t>4.8.2. Quel est le numéro de téléphone alternatif du membre ? (Si disponible)</t>
+  </si>
+  <si>
     <t>collected</t>
   </si>
   <si>
@@ -461,6 +506,24 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Non</t>
   </si>
   <si>
     <t>M</t>
@@ -781,9 +844,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -817,11 +880,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -829,6 +892,28 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -842,9 +927,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -855,16 +940,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -879,31 +979,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -917,6 +1000,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -924,36 +1008,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -961,6 +1015,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -994,25 +1057,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,7 +1093,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,55 +1111,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1102,7 +1135,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,13 +1189,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,49 +1237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1263,11 +1326,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1283,15 +1344,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1328,6 +1380,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1352,152 +1415,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1533,6 +1596,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1543,6 +1607,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1560,6 +1628,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1880,10 +1949,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1931,7 +2000,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="28" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1946,7 +2015,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="35" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1962,15 +2031,15 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
@@ -1987,7 +2056,7 @@
       <c r="N2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="31"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -2008,8 +2077,8 @@
       <c r="J3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
       <c r="M3" t="b">
         <v>1</v>
       </c>
@@ -2036,8 +2105,8 @@
       <c r="J4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
       <c r="M4" t="b">
         <v>1</v>
       </c>
@@ -2066,8 +2135,8 @@
       <c r="J5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
       <c r="M5" t="b">
         <v>1</v>
       </c>
@@ -2094,8 +2163,8 @@
       <c r="J6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
       <c r="M6" t="b">
         <v>1</v>
       </c>
@@ -2122,8 +2191,8 @@
       <c r="J7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
       <c r="M7" t="b">
         <v>1</v>
       </c>
@@ -2147,8 +2216,8 @@
       <c r="J8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
       <c r="M8" t="b">
         <v>1</v>
       </c>
@@ -2172,8 +2241,8 @@
       <c r="J9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
       <c r="M9" t="b">
         <v>1</v>
       </c>
@@ -2195,8 +2264,8 @@
       <c r="J10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
       <c r="M10" t="b">
         <v>1</v>
       </c>
@@ -2221,8 +2290,8 @@
       <c r="J11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
       <c r="M11" t="b">
         <v>1</v>
       </c>
@@ -2249,8 +2318,8 @@
       <c r="J12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
       <c r="M12" t="b">
         <v>1</v>
       </c>
@@ -2283,8 +2352,8 @@
       <c r="J13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
       <c r="M13" t="b">
         <v>1</v>
       </c>
@@ -2315,8 +2384,8 @@
       <c r="J14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
       <c r="M14" t="b">
         <v>1</v>
       </c>
@@ -2344,8 +2413,8 @@
       <c r="J15" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
       <c r="M15" t="b">
         <v>1</v>
       </c>
@@ -2370,8 +2439,8 @@
       <c r="J16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
       <c r="M16" t="b">
         <v>1</v>
       </c>
@@ -2396,8 +2465,8 @@
       <c r="J17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
       <c r="M17" t="b">
         <v>1</v>
       </c>
@@ -2422,8 +2491,8 @@
       <c r="J18" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
       <c r="M18" t="b">
         <v>1</v>
       </c>
@@ -2445,8 +2514,8 @@
       <c r="J19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
       <c r="M19" t="b">
         <v>1</v>
       </c>
@@ -2455,271 +2524,363 @@
       </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20" t="s">
+      <c r="G20" s="21"/>
+      <c r="H20" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20" t="s">
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20" t="s">
+      <c r="G21" s="21"/>
+      <c r="H21" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-    </row>
-    <row r="22" s="15" customFormat="1" spans="1:14">
-      <c r="A22" s="21" t="s">
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+    </row>
+    <row r="22" s="15" customFormat="1" spans="1:17">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="E22" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="G22" s="23"/>
+      <c r="H22" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="15" t="s">
+      <c r="I22" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="J22" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+    </row>
+    <row r="23" s="15" customFormat="1" spans="1:17">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="N22" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" s="16" customFormat="1" spans="1:14">
-      <c r="A23" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="16" t="s">
+      <c r="E23" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="I23" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="J23" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="P23" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="N23" s="16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" s="16" customFormat="1" spans="1:17">
-      <c r="A24" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="16" t="s">
+      <c r="Q23" s="23"/>
+    </row>
+    <row r="24" s="15" customFormat="1" spans="1:17">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="I24" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="I24" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="N24" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" s="16" customFormat="1" spans="1:17">
-      <c r="A25" s="22" t="s">
-        <v>114</v>
+      <c r="J24" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="P24" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q24" s="23"/>
+    </row>
+    <row r="25" s="16" customFormat="1" spans="1:14">
+      <c r="A25" s="24" t="s">
+        <v>129</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E25" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N25" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" s="17" customFormat="1" spans="1:14">
+      <c r="A26" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N26" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" s="17" customFormat="1" spans="1:17">
+      <c r="A27" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="N27" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" s="17" customFormat="1" spans="1:17">
+      <c r="A28" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H28" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="N28" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" s="17" customFormat="1" spans="1:17">
+      <c r="A29" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="D29" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="N29" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" s="18" customFormat="1" spans="1:14">
+      <c r="A30" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="J25" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="N25" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" s="16" customFormat="1" spans="1:17">
-      <c r="A26" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="16" t="s">
+      <c r="D30" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="N26" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" s="17" customFormat="1" spans="1:14">
-      <c r="A27" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="N27" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="1"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="1"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
+      <c r="H30" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="N30" s="18" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="1"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="1"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1"/>
@@ -2744,6 +2905,15 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -2755,10 +2925,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2775,7 +2945,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2791,93 +2961,95 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" s="3"/>
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="F3" s="3"/>
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>157</v>
+      <c r="B6" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2885,16 +3057,16 @@
         <v>60</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2902,16 +3074,16 @@
         <v>60</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2919,16 +3091,16 @@
         <v>60</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2936,16 +3108,16 @@
         <v>60</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2953,16 +3125,16 @@
         <v>60</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2970,118 +3142,118 @@
         <v>60</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>185</v>
+      <c r="A13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" t="s">
-        <v>188</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>189</v>
+      <c r="A14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="D15" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D16" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C16" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>199</v>
+      <c r="B17" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C17" t="s">
+        <v>212</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>203</v>
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" t="s">
+        <v>216</v>
       </c>
       <c r="D18" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3089,16 +3261,16 @@
         <v>95</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="D19" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3106,16 +3278,16 @@
         <v>95</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>211</v>
+        <v>223</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>224</v>
       </c>
       <c r="D20" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3123,16 +3295,16 @@
         <v>95</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="D21" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3140,16 +3312,16 @@
         <v>95</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>219</v>
+        <v>231</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="D22" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3157,16 +3329,16 @@
         <v>95</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="D23" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3174,69 +3346,87 @@
         <v>95</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="D24" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
         <v>95</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>231</v>
+        <v>243</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>244</v>
       </c>
       <c r="D25" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:6">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B26" t="s">
-        <v>234</v>
-      </c>
-      <c r="C26" t="s">
-        <v>179</v>
+      <c r="B26" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>248</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F26" s="10"/>
+        <v>250</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="8"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="A27" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="8"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="A28" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="8"/>
@@ -3250,9 +3440,9 @@
       <c r="A30" s="8"/>
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="8"/>
@@ -3268,7 +3458,7 @@
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="9"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="8"/>
@@ -3284,7 +3474,7 @@
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="8"/>
@@ -3318,23 +3508,33 @@
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
     </row>
-    <row r="40" spans="6:6">
+    <row r="39" spans="1:6">
+      <c r="A39" s="8"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="8"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
       <c r="F40" s="10"/>
-    </row>
-    <row r="41" spans="6:6">
-      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="6:6">
       <c r="F42" s="10"/>
     </row>
     <row r="43" spans="6:6">
-      <c r="F43" s="9"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="6:6">
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="6:6">
-      <c r="F45" s="10"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="6:6">
       <c r="F46" s="10"/>
@@ -3344,6 +3544,12 @@
     </row>
     <row r="48" spans="6:6">
       <c r="F48" s="10"/>
+    </row>
+    <row r="49" spans="6:6">
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="6:6">
+      <c r="F50" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3371,30 +3577,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>238</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Fix editing Internal InMig, External InMig and ChangeHead - dont validate with recently created residency or head relationship - Make memberName,memberGender,memberDog readonly when Externally Inmigrating a Member with REENTRY
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/ext_inmigration_form.xlsx
+++ b/app/src/main/res/raw/ext_inmigration_form.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="321">
   <si>
     <t>group</t>
   </si>
@@ -205,6 +205,54 @@
     <t xml:space="preserve">2.4. የአባቱ ስም  </t>
   </si>
   <si>
+    <t>migration</t>
+  </si>
+  <si>
+    <t>migrationType</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>migtypes</t>
+  </si>
+  <si>
+    <t>2.5. Immigration Type</t>
+  </si>
+  <si>
+    <t>2.5. Tipo de Imigração</t>
+  </si>
+  <si>
+    <t>2.5. Type d'immigration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5. የመግቢያ አይነት  </t>
+  </si>
+  <si>
+    <t>selected_only</t>
+  </si>
+  <si>
+    <t>extMigrationType</t>
+  </si>
+  <si>
+    <t>extmigtypes</t>
+  </si>
+  <si>
+    <t>2.5.1. External Inmigration type</t>
+  </si>
+  <si>
+    <t>2.5.1. Tipo de Imigração Externa</t>
+  </si>
+  <si>
+    <t>2.5.1. Type d'immigration externe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5.1. ውጫዊ መግቢያ አይነት  </t>
+  </si>
+  <si>
+    <t>${migrationType} = 'XEN'</t>
+  </si>
+  <si>
     <t>memberName</t>
   </si>
   <si>
@@ -220,12 +268,12 @@
     <t xml:space="preserve">3.1. የአባሉ ስም  </t>
   </si>
   <si>
+    <t>${extMigrationType} = 'REENTRY'</t>
+  </si>
+  <si>
     <t>memberGender</t>
   </si>
   <si>
-    <t>select</t>
-  </si>
-  <si>
     <t>genders</t>
   </si>
   <si>
@@ -277,51 +325,6 @@
     <t xml:space="preserve">3.4. ከየቤተሰቡ አለቃ ጋር ያለው ዝምድና  </t>
   </si>
   <si>
-    <t>migration</t>
-  </si>
-  <si>
-    <t>migrationType</t>
-  </si>
-  <si>
-    <t>migtypes</t>
-  </si>
-  <si>
-    <t>3.5. Immigration Type</t>
-  </si>
-  <si>
-    <t>3.5. Tipo de Imigração</t>
-  </si>
-  <si>
-    <t>3.5. Type d'immigration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.5. የመግቢያ አይነት  </t>
-  </si>
-  <si>
-    <t>selected_only</t>
-  </si>
-  <si>
-    <t>extMigrationType</t>
-  </si>
-  <si>
-    <t>extmigtypes</t>
-  </si>
-  <si>
-    <t>3.5.1. External Inmigration type</t>
-  </si>
-  <si>
-    <t>3.5.1. Tipo de Imigração Externa</t>
-  </si>
-  <si>
-    <t>3.5.1. Type d'immigration externe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.5.1. ውጫዊ መግቢያ አይነት  </t>
-  </si>
-  <si>
-    <t>${migrationType} = 'XEN'</t>
-  </si>
-  <si>
     <t>originCode</t>
   </si>
   <si>
@@ -335,9 +338,6 @@
   </si>
   <si>
     <t xml:space="preserve">4.1. የመነሻ ቤተሰብ ኮድ  </t>
-  </si>
-  <si>
-    <t>${extMigrationType} = 'REENTRY'</t>
   </si>
   <si>
     <t>originOther</t>
@@ -1020,9 +1020,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
@@ -1057,16 +1057,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1074,29 +1067,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1110,40 +1080,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1157,21 +1095,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1194,7 +1126,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1203,6 +1157,52 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1234,7 +1234,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1246,7 +1270,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1258,13 +1330,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1276,13 +1372,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1294,109 +1390,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1414,7 +1408,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1492,30 +1492,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1540,21 +1516,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1569,8 +1530,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1589,151 +1550,190 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2155,8 +2155,8 @@
   <sheetPr/>
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -2174,6 +2174,7 @@
     <col min="12" max="12" width="16.2666666666667" customWidth="1"/>
     <col min="13" max="13" width="14.1809523809524" customWidth="1"/>
     <col min="14" max="14" width="9.26666666666667" customWidth="1"/>
+    <col min="15" max="15" width="32.1428571428571" customWidth="1"/>
     <col min="16" max="16" width="31" customWidth="1"/>
     <col min="17" max="17" width="13.4571428571429" customWidth="1"/>
   </cols>
@@ -2427,210 +2428,219 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="4:14">
+    <row r="8" spans="1:17">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L8" s="33"/>
       <c r="M8" s="33"/>
       <c r="N8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="4:14">
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L9" s="33"/>
       <c r="M9" s="33"/>
       <c r="N9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="1"/>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15">
       <c r="D10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K10" s="32" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L10" s="33"/>
       <c r="M10" s="33"/>
       <c r="N10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="1"/>
+      <c r="O10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="4:15">
       <c r="D11" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K11" s="32" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L11" s="33"/>
       <c r="M11" s="33"/>
       <c r="N11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="O11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1"/>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L12" s="33"/>
       <c r="M12" s="33"/>
       <c r="N12" t="b">
         <v>1</v>
       </c>
-      <c r="O12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="O12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K13" s="32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L13" s="33"/>
       <c r="M13" s="33"/>
       <c r="N13" t="b">
         <v>1</v>
       </c>
-      <c r="O13" t="b">
-        <v>1</v>
-      </c>
-      <c r="P13" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1"/>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K14" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
@@ -2641,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2670,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -2708,7 +2718,7 @@
         <v>106</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="H17" t="s">
         <v>107</v>
@@ -2734,7 +2744,7 @@
         <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
         <v>112</v>
@@ -2794,7 +2804,7 @@
         <v>123</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>124</v>
@@ -2832,7 +2842,7 @@
         <v>130</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>131</v>
@@ -2866,7 +2876,7 @@
         <v>135</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>136</v>
@@ -3288,7 +3298,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>190</v>
@@ -3309,7 +3319,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>195</v>
@@ -3330,7 +3340,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>200</v>
@@ -3353,7 +3363,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>206</v>
@@ -3373,7 +3383,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>211</v>
@@ -3393,7 +3403,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>216</v>
@@ -3413,7 +3423,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>221</v>
@@ -3433,7 +3443,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>226</v>
@@ -3453,7 +3463,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>231</v>
@@ -3473,7 +3483,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>236</v>
@@ -3493,7 +3503,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>241</v>
@@ -3513,7 +3523,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>246</v>
@@ -3533,7 +3543,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>251</v>
@@ -3553,7 +3563,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>256</v>
@@ -3573,7 +3583,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>261</v>

</xml_diff>

<commit_message>
- Add initial Household Institution support   - Add new variables to Household Form   - Add new icons and update views   - Update some FormUtil used on Institutions to handle correctly HeadRelationships - Remove the non-used variable secHeadCode
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/ext_inmigration_form.xlsx
+++ b/app/src/main/res/raw/ext_inmigration_form.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="322">
   <si>
     <t>group</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t xml:space="preserve">3.4. ከየቤተሰቡ አለቃ ጋር ያለው ዝምድና  </t>
+  </si>
+  <si>
+    <t>call:isInstitutionalHousehold() = 'false'</t>
   </si>
   <si>
     <t>originCode</t>
@@ -1020,10 +1023,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1057,14 +1060,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1072,16 +1067,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1094,8 +1081,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1104,6 +1108,66 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1133,63 +1197,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1198,13 +1208,6 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1219,7 +1222,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1234,7 +1237,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC5D9F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1252,61 +1399,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1318,103 +1417,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1492,11 +1501,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1512,6 +1527,45 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1536,51 +1590,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1592,152 +1601,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1838,6 +1847,9 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2155,8 +2167,8 @@
   <sheetPr/>
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -2593,7 +2605,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:16">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
         <v>85</v>
@@ -2621,26 +2633,29 @@
       <c r="N13" t="b">
         <v>1</v>
       </c>
+      <c r="P13" s="45" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1"/>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K14" s="32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
@@ -2657,22 +2672,22 @@
     <row r="15" spans="1:16">
       <c r="A15" s="1"/>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K15" s="32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L15" s="33"/>
       <c r="M15" s="33"/>
@@ -2686,22 +2701,22 @@
     <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K16" s="32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
@@ -2715,22 +2730,22 @@
     <row r="17" spans="1:14">
       <c r="A17" s="1"/>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
         <v>80</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K17" s="32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
@@ -2741,25 +2756,25 @@
     <row r="18" spans="1:14">
       <c r="A18" s="1"/>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
         <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K18" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -2770,22 +2785,22 @@
     <row r="19" spans="1:16">
       <c r="A19" s="1"/>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K19" s="32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L19" s="33"/>
       <c r="M19" s="33"/>
@@ -2793,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="P19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2801,26 +2816,26 @@
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>53</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G20" s="24"/>
       <c r="H20" s="24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L20" s="35"/>
       <c r="M20" s="35"/>
@@ -2829,7 +2844,7 @@
       </c>
       <c r="O20" s="24"/>
       <c r="P20" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
@@ -2839,26 +2854,26 @@
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
       <c r="D21" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>53</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G21" s="24"/>
       <c r="H21" s="24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I21" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="J21" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="J21" s="24" t="s">
-        <v>132</v>
-      </c>
       <c r="K21" s="34" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L21" s="35"/>
       <c r="M21" s="35"/>
@@ -2873,25 +2888,25 @@
     <row r="22" s="19" customFormat="1" spans="1:14">
       <c r="A22" s="25"/>
       <c r="D22" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>53</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K22" s="36" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="L22" s="37"/>
       <c r="M22" s="37"/>
@@ -2902,22 +2917,22 @@
     <row r="23" s="19" customFormat="1" spans="1:17">
       <c r="A23" s="25"/>
       <c r="D23" s="19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K23" s="36" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L23" s="37"/>
       <c r="M23" s="37"/>
@@ -2925,64 +2940,64 @@
         <v>1</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" s="19" customFormat="1" spans="1:17">
       <c r="A24" s="25"/>
       <c r="D24" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K24" s="36" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L24" s="37"/>
       <c r="M24" s="37"/>
       <c r="P24" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" s="20" customFormat="1" spans="1:15">
       <c r="A25" s="26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K25" s="38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L25" s="39"/>
       <c r="M25" s="39"/>
@@ -2995,25 +3010,25 @@
     </row>
     <row r="26" s="21" customFormat="1" spans="1:15">
       <c r="A26" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J26" s="21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K26" s="40" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
@@ -3026,25 +3041,25 @@
     </row>
     <row r="27" s="21" customFormat="1" spans="1:18">
       <c r="A27" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K27" s="40" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
@@ -3057,25 +3072,25 @@
     </row>
     <row r="28" s="21" customFormat="1" spans="1:18">
       <c r="A28" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K28" s="40" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
@@ -3088,25 +3103,25 @@
     </row>
     <row r="29" s="21" customFormat="1" spans="1:18">
       <c r="A29" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K29" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
@@ -3119,25 +3134,25 @@
     </row>
     <row r="30" s="22" customFormat="1" spans="1:15">
       <c r="A30" s="28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>20</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K30" s="42" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L30" s="43"/>
       <c r="M30" s="43"/>
@@ -3236,7 +3251,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -3256,43 +3271,43 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -3301,19 +3316,19 @@
         <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -3322,19 +3337,19 @@
         <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -3343,22 +3358,22 @@
         <v>86</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3366,19 +3381,19 @@
         <v>86</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3386,19 +3401,19 @@
         <v>86</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3406,19 +3421,19 @@
         <v>86</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3426,19 +3441,19 @@
         <v>86</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3446,19 +3461,19 @@
         <v>86</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3466,19 +3481,19 @@
         <v>86</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3486,19 +3501,19 @@
         <v>86</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3506,19 +3521,19 @@
         <v>86</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3526,19 +3541,19 @@
         <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D15" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3546,19 +3561,19 @@
         <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3566,19 +3581,19 @@
         <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3586,220 +3601,220 @@
         <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C18" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D18" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D20" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D21" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D23" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D24" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D25" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D27" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D28" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G28" s="10"/>
     </row>
@@ -3974,36 +3989,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>